<commit_message>
Completed the outline and Data Items section of project plannign
</commit_message>
<xml_diff>
--- a/RobotWriter2025/MMME3085 Project Prep Template25-26.xlsx
+++ b/RobotWriter2025/MMME3085 Project Prep Template25-26.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofnottm-my.sharepoint.com/personal/louise_brown_nottingham_ac_uk/Documents/Documents/Mechatronics/MMME3085 2024-2025/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\OneDrive\Documents\Uni documents\mechatronics\Robot Writer Project\RobotWriter2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{15D13596-4042-40F7-896D-0FE0C06DCFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1888E69-EC62-4B2D-BBAB-9AC62C6AE8FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AABDE51-9522-4E73-809B-119D71EBD1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2595" windowWidth="29040" windowHeight="15840" xr2:uid="{BEAF5B25-FF5C-42C7-9ED0-BDEC0A921434}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEAF5B25-FF5C-42C7-9ED0-BDEC0A921434}"/>
   </bookViews>
   <sheets>
     <sheet name="Marking" sheetId="1" r:id="rId1"/>
@@ -571,63 +571,21 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -636,6 +594,48 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1268,7 +1268,7 @@
   </sheetPr>
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C28" sqref="C28:S28"/>
     </sheetView>
   </sheetViews>
@@ -1280,26 +1280,26 @@
   <sheetData>
     <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
       <c r="T1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1307,119 +1307,119 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
     </row>
     <row r="6" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="29"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="40"/>
       <c r="T6" s="10" t="str">
         <f>IF(C6="","No Selection","OK")</f>
         <v>No Selection</v>
@@ -1430,95 +1430,95 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
     </row>
     <row r="10" spans="1:21" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
       <c r="T10" t="str">
         <f>IF(C10="","No Selection","OK")</f>
         <v>No Selection</v>
@@ -1529,95 +1529,95 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
     </row>
     <row r="14" spans="1:21" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
       <c r="T14" s="10" t="str">
         <f>IF(C14="","No Selection","OK")</f>
         <v>No Selection</v>
@@ -1628,95 +1628,95 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
     </row>
     <row r="18" spans="1:21" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
       <c r="T18" s="10" t="str">
         <f>IF(C18="","No Selection","OK")</f>
         <v>No Selection</v>
@@ -1727,95 +1727,95 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
     </row>
     <row r="22" spans="1:21" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="31"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="28"/>
       <c r="T22" s="10" t="str">
         <f>IF(C22="","No Selection","OK")</f>
         <v>No Selection</v>
@@ -1826,49 +1826,49 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
     </row>
     <row r="24" spans="1:21" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="34"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="31"/>
       <c r="T24" s="10" t="str">
         <f>IF(C24="","No Selection","OK")</f>
         <v>No Selection</v>
@@ -1879,97 +1879,97 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="26"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
     </row>
     <row r="28" spans="1:21" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
       <c r="T28" s="10" t="str">
         <f>IF(C28="","No Selection","OK")</f>
         <v>OK</v>
@@ -2024,107 +2024,107 @@
       <c r="T30" s="9"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="26"/>
-      <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
     </row>
     <row r="33" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="39"/>
-      <c r="R33" s="39"/>
-      <c r="S33" s="39"/>
-      <c r="T33" s="40"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="25"/>
+      <c r="S33" s="25"/>
+      <c r="T33" s="26"/>
     </row>
     <row r="34" spans="1:20" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="36"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="T34" s="37"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B34:T34"/>
-    <mergeCell ref="A12:T12"/>
-    <mergeCell ref="A13:T13"/>
-    <mergeCell ref="C14:S14"/>
-    <mergeCell ref="A15:T15"/>
-    <mergeCell ref="A32:T32"/>
-    <mergeCell ref="B33:T33"/>
-    <mergeCell ref="A27:T27"/>
-    <mergeCell ref="C28:S28"/>
+    <mergeCell ref="A5:T5"/>
+    <mergeCell ref="A7:T7"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="A3:T3"/>
+    <mergeCell ref="A4:T4"/>
+    <mergeCell ref="C6:S6"/>
     <mergeCell ref="A8:T8"/>
     <mergeCell ref="A9:T9"/>
     <mergeCell ref="C10:S10"/>
@@ -2141,15 +2141,15 @@
     <mergeCell ref="C24:S24"/>
     <mergeCell ref="A23:T23"/>
     <mergeCell ref="A26:T26"/>
-    <mergeCell ref="A5:T5"/>
-    <mergeCell ref="A7:T7"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="A3:T3"/>
-    <mergeCell ref="A4:T4"/>
-    <mergeCell ref="C6:S6"/>
+    <mergeCell ref="B34:T34"/>
+    <mergeCell ref="A12:T12"/>
+    <mergeCell ref="A13:T13"/>
+    <mergeCell ref="C14:S14"/>
+    <mergeCell ref="A15:T15"/>
+    <mergeCell ref="A32:T32"/>
+    <mergeCell ref="B33:T33"/>
+    <mergeCell ref="A27:T27"/>
+    <mergeCell ref="C28:S28"/>
   </mergeCells>
   <conditionalFormatting sqref="T6">
     <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="OK">
@@ -2267,8 +2267,8 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>